<commit_message>
change namespace and add stage actors
</commit_message>
<xml_diff>
--- a/StaticData/BattleScene.xlsx
+++ b/StaticData/BattleScene.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BattleScene" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>Data</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -153,6 +153,22 @@
   </si>
   <si>
     <t>Int32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>All</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EntityList</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>List&lt;StageActor{Uid:Int32,Rid:Int32,Level:Int32,PosX:Int32,PosY:Int32}&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101,1,4,5,3 | 102,1,4,5,1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -481,7 +497,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -565,10 +581,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -577,9 +593,10 @@
     <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="76.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -587,7 +604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -606,8 +623,11 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -626,8 +646,11 @@
       <c r="F3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -646,23 +669,26 @@
       <c r="F4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -680,11 +706,15 @@
       </c>
       <c r="F8" t="s">
         <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -692,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>